<commit_message>
modified:   01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx 	modified:   03_Advanced_Internet_Programming/Assignments/Lab01/001.FilipeMatos/index.html 	03_Advanced_Internet_Programming/Assignments/Lab02/ 	03_Advanced_Internet_Programming/Frontend/ 	03_Advanced_Internet_Programming/Lectures/00-Presentation.pdf 	03_Advanced_Internet_Programming/Lectures/01-Review.pdf 	03_Advanced_Internet_Programming/Lectures/02-ModernJS-HTML5.pdf 	03_Advanced_Internet_Programming/Lectures/resources/
</commit_message>
<xml_diff>
--- a/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx
+++ b/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/201600728_estudantes_ips_pt/Documents/02. MEEC/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{0AC68C7C-9C0E-40AA-A00B-9B85F49A533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75E46B57-A7AB-4D0A-877E-F933FB105A52}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{0AC68C7C-9C0E-40AA-A00B-9B85F49A533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF7C2C20-7D15-4848-9BCC-CCF49BA8A8C5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{DEA98590-6CE2-4FA0-BAE4-FD939EE61D3A}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{DEA98590-6CE2-4FA0-BAE4-FD939EE61D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="2" r:id="rId1"/>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="123">
   <si>
     <t>VendaID</t>
   </si>
@@ -399,6 +421,12 @@
   </si>
   <si>
     <t>AproxEscalaClienteInf</t>
+  </si>
+  <si>
+    <t>9.1 - Filter por Categoria e Região</t>
+  </si>
+  <si>
+    <t>9.2 - Filter por Vendas deste mês com a data atual</t>
   </si>
 </sst>
 </file>
@@ -540,7 +568,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -602,9 +630,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -738,9 +763,24 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}" name="Vendas" displayName="Vendas" ref="A1:V37" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:V37" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}"/>
+  <autoFilter ref="A1:V37" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="Norte"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="Higiene"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00E18295-A8E0-4DEE-A175-C2D1DE60A124}" name="VendaID" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{2A9F5B6B-8F27-432C-B2C7-24A3E549C555}" name="Data" dataDxfId="20"/>
@@ -1079,13 +1119,13 @@
     <sheetView workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>78</v>
       </c>
@@ -1093,7 +1133,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1101,7 +1141,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1149,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1157,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +1165,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1133,7 +1173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1141,7 +1181,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1149,7 +1189,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1157,7 +1197,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1165,7 +1205,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1185,21 +1225,21 @@
     <sheetView topLeftCell="J2" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
       <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="15" width="20" style="10" customWidth="1"/>
-    <col min="16" max="16" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="26.81640625" customWidth="1"/>
-    <col min="20" max="20" width="25.6328125" customWidth="1"/>
+    <col min="16" max="16" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.85546875" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1260,14 +1300,14 @@
       <c r="T1" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="U1" s="24" t="s">
+      <c r="U1" s="23" t="s">
         <v>117</v>
       </c>
       <c r="V1" s="14" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -1320,7 +1360,7 @@
       </c>
       <c r="P2" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1338,10 +1378,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U2" s="23"/>
-      <c r="V2" s="23"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+    </row>
+    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1394,7 +1434,7 @@
       </c>
       <c r="P3" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="Q3" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1412,10 +1452,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+    </row>
+    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1468,7 +1508,7 @@
       </c>
       <c r="P4" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="Q4" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1486,10 +1526,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U4" s="23"/>
-      <c r="V4" s="23"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+    </row>
+    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -1542,7 +1582,7 @@
       </c>
       <c r="P5" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="Q5" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1560,10 +1600,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+    </row>
+    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1616,7 +1656,7 @@
       </c>
       <c r="P6" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="Q6" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1634,10 +1674,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+    </row>
+    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
@@ -1690,7 +1730,7 @@
       </c>
       <c r="P7" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="Q7" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1708,10 +1748,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+    </row>
+    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
@@ -1764,7 +1804,7 @@
       </c>
       <c r="P8" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="Q8" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1782,10 +1822,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -1838,7 +1878,7 @@
       </c>
       <c r="P9" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="Q9" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1856,10 +1896,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U9" s="23"/>
-      <c r="V9" s="23"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+    </row>
+    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
@@ -1912,7 +1952,7 @@
       </c>
       <c r="P10" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="Q10" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1930,10 +1970,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Ouro</v>
       </c>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+    </row>
+    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
@@ -1986,7 +2026,7 @@
       </c>
       <c r="P11" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Q11" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2004,10 +2044,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+    </row>
+    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>42</v>
       </c>
@@ -2060,7 +2100,7 @@
       </c>
       <c r="P12" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="Q12" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2078,10 +2118,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U12" s="23"/>
-      <c r="V12" s="23"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>44</v>
       </c>
@@ -2134,7 +2174,7 @@
       </c>
       <c r="P13" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="Q13" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2152,10 +2192,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U13" s="23"/>
-      <c r="V13" s="23"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>45</v>
       </c>
@@ -2208,7 +2248,7 @@
       </c>
       <c r="P14" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Q14" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2226,10 +2266,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U14" s="23"/>
-      <c r="V14" s="23"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+    </row>
+    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>48</v>
       </c>
@@ -2282,7 +2322,7 @@
       </c>
       <c r="P15" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="Q15" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2300,10 +2340,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+    </row>
+    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>51</v>
       </c>
@@ -2356,7 +2396,7 @@
       </c>
       <c r="P16" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Q16" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2374,10 +2414,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U16" s="23"/>
-      <c r="V16" s="23"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+    </row>
+    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
@@ -2430,7 +2470,7 @@
       </c>
       <c r="P17" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Q17" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2448,10 +2488,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U17" s="23"/>
-      <c r="V17" s="23"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+    </row>
+    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>53</v>
       </c>
@@ -2504,7 +2544,7 @@
       </c>
       <c r="P18" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="Q18" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2522,10 +2562,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U18" s="23"/>
-      <c r="V18" s="23"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+    </row>
+    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>55</v>
       </c>
@@ -2578,7 +2618,7 @@
       </c>
       <c r="P19" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="Q19" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2596,10 +2636,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Platina</v>
       </c>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+    </row>
+    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>57</v>
       </c>
@@ -2652,7 +2692,7 @@
       </c>
       <c r="P20" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="Q20" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2670,10 +2710,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U20" s="23"/>
-      <c r="V20" s="23"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>58</v>
       </c>
@@ -2726,7 +2766,7 @@
       </c>
       <c r="P21" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="Q21" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2744,10 +2784,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Ouro</v>
       </c>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+    </row>
+    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>59</v>
       </c>
@@ -2800,7 +2840,7 @@
       </c>
       <c r="P22" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="Q22" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2818,10 +2858,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Platina</v>
       </c>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>60</v>
       </c>
@@ -2874,7 +2914,7 @@
       </c>
       <c r="P23" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q23" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2892,10 +2932,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U23" s="23"/>
-      <c r="V23" s="23"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+    </row>
+    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>61</v>
       </c>
@@ -2948,7 +2988,7 @@
       </c>
       <c r="P24" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q24" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2966,10 +3006,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U24" s="23"/>
-      <c r="V24" s="23"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+    </row>
+    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>62</v>
       </c>
@@ -3022,7 +3062,7 @@
       </c>
       <c r="P25" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="Q25" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3040,10 +3080,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+    </row>
+    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>63</v>
       </c>
@@ -3096,7 +3136,7 @@
       </c>
       <c r="P26" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="Q26" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3114,10 +3154,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U26" s="23"/>
-      <c r="V26" s="23"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+    </row>
+    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>64</v>
       </c>
@@ -3170,7 +3210,7 @@
       </c>
       <c r="P27" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="Q27" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3188,10 +3228,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U27" s="23"/>
-      <c r="V27" s="23"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+    </row>
+    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>65</v>
       </c>
@@ -3244,7 +3284,7 @@
       </c>
       <c r="P28" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Q28" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3262,10 +3302,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U28" s="23"/>
-      <c r="V28" s="23"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>66</v>
       </c>
@@ -3318,7 +3358,7 @@
       </c>
       <c r="P29" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="Q29" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3336,10 +3376,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U29" s="23"/>
-      <c r="V29" s="23"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
+    </row>
+    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>67</v>
       </c>
@@ -3392,7 +3432,7 @@
       </c>
       <c r="P30" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q30" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3410,10 +3450,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U30" s="23"/>
-      <c r="V30" s="23"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
+    </row>
+    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>68</v>
       </c>
@@ -3466,7 +3506,7 @@
       </c>
       <c r="P31" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="Q31" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3484,10 +3524,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U31" s="23"/>
-      <c r="V31" s="23"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
+    </row>
+    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
@@ -3540,7 +3580,7 @@
       </c>
       <c r="P32" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="Q32" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3558,10 +3598,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U32" s="23"/>
-      <c r="V32" s="23"/>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
+    </row>
+    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>72</v>
       </c>
@@ -3614,7 +3654,7 @@
       </c>
       <c r="P33" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="Q33" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3632,10 +3672,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Prata</v>
       </c>
-      <c r="U33" s="23"/>
-      <c r="V33" s="23"/>
-    </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+    </row>
+    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
@@ -3688,7 +3728,7 @@
       </c>
       <c r="P34" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Q34" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3706,10 +3746,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U34" s="23"/>
-      <c r="V34" s="23"/>
-    </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
+    </row>
+    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>74</v>
       </c>
@@ -3762,7 +3802,7 @@
       </c>
       <c r="P35" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q35" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3780,10 +3820,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U35" s="23"/>
-      <c r="V35" s="23"/>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+    </row>
+    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>76</v>
       </c>
@@ -3836,7 +3876,7 @@
       </c>
       <c r="P36" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q36" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3854,10 +3894,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U36" s="23"/>
-      <c r="V36" s="23"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
+    </row>
+    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>77</v>
       </c>
@@ -3910,7 +3950,7 @@
       </c>
       <c r="P37" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q37" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3928,10 +3968,10 @@
         <f>_xlfn.XLOOKUP(Vendas[[#This Row],[Total]],Análise!$R$4:$R$7,Análise!$S$4:$S$7,,-1)</f>
         <v>Bronze</v>
       </c>
-      <c r="U37" s="23"/>
-      <c r="V37" s="23"/>
-    </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K40" s="18"/>
     </row>
   </sheetData>
@@ -3945,25 +3985,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D0DA00-7E98-40C2-8941-409BD587D4AF}">
-  <dimension ref="B2:S20"/>
+  <dimension ref="B2:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:S7"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q26" sqref="Q26"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.26953125" customWidth="1"/>
-    <col min="7" max="7" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" customWidth="1"/>
-    <col min="11" max="13" width="20.54296875" customWidth="1"/>
-    <col min="17" max="17" width="25.1796875" customWidth="1"/>
+    <col min="11" max="13" width="20.5703125" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>90</v>
       </c>
@@ -3977,7 +4017,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -4011,7 +4051,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -4048,7 +4088,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>47</v>
       </c>
@@ -4085,7 +4125,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -4122,7 +4162,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="R7" s="10">
         <v>350</v>
@@ -4131,10 +4171,10 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="2:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>91</v>
       </c>
@@ -4144,11 +4184,11 @@
       <c r="J9" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="Q9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q9" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>71</v>
       </c>
@@ -4176,7 +4216,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
@@ -4200,8 +4240,12 @@
         <f>_xlfn.XLOOKUP(K11,Vendas[Total],Vendas[Produto],,0)</f>
         <v>Papel A4 500</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q11" s="10" cm="1">
+        <f t="array" ref="Q11:Q15">_xlfn._xlws.FILTER(Vendas[Quantidade],((Vendas[Categoria]="Higiene")*(Vendas[Região]="Norte")))</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
@@ -4225,8 +4269,11 @@
         <f>_xlfn.XLOOKUP(K12,Vendas[Total],Vendas[Produto],,0)</f>
         <v>Toalhitas</v>
       </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q12" s="21">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
@@ -4250,8 +4297,11 @@
         <f>_xlfn.XLOOKUP(K13,Vendas[Total],Vendas[Produto],,0)</f>
         <v>Papel A4 500</v>
       </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q13" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -4260,22 +4310,30 @@
         <v>13</v>
       </c>
       <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q14" s="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="Q15" s="21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="Q16" s="21"/>
+    </row>
+    <row r="17" spans="2:17" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>92</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="Q17" s="21"/>
+    </row>
+    <row r="18" spans="2:17" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -4290,8 +4348,11 @@
         <f>AVERAGEIFS(Vendas[Total],Vendas[Categoria],B20,Vendas[Trimestre],1)</f>
         <v>64.716166666666666</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="Q18" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -4300,8 +4361,9 @@
         <v>84.802349999999976</v>
       </c>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="Q19" s="21"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -4310,6 +4372,31 @@
         <v>67.928937499999989</v>
       </c>
       <c r="F20" s="5"/>
+      <c r="Q20" s="21"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q21" s="21"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q22" s="21"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q23" s="21"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q24" s="21"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q25" s="21"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q26" s="21"/>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q27" s="21"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q28" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
modified:   01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx  	modified:   02_Programming_Mobile_Devices/Assignments/lab01/bin/lab01.dart  	modified:   02_Programming_Mobile_Devices/Assignments/lab01/lib/lab01.dart  	modified:   02_Programming_Mobile_Devices/Assignments/lab01/pubspec.yaml  	modified:   03_Advanced_Internet_Programming/Assignments/Lab02/index.html  	modified:   03_Advanced_Internet_Programming/Assignments/Lab02/resources/scripts/Task.js  	modified:   03_Advanced_Internet_Programming/Assignments/Lab02/resources/scripts/main.js  	modified:   03_Advanced_Internet_Programming/Assignments/Lab02/resources/styles/main.css
</commit_message>
<xml_diff>
--- a/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx
+++ b/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/dataset_vendas_alunos v1.0.xlsx
@@ -2,16 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsetubal-my.sharepoint.com/personal/201600728_estudantes_ips_pt/Documents/02. MEEC/01_Data_Analysis/Assignments/FuncoesExcel_Vendas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="8_{0AC68C7C-9C0E-40AA-A00B-9B85F49A533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF7C2C20-7D15-4848-9BCC-CCF49BA8A8C5}"/>
+  <xr:revisionPtr revIDLastSave="329" documentId="8_{0AC68C7C-9C0E-40AA-A00B-9B85F49A533F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE818EE-00DF-4B79-9424-A63E5DF34454}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{DEA98590-6CE2-4FA0-BAE4-FD939EE61D3A}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{DEA98590-6CE2-4FA0-BAE4-FD939EE61D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Dicionário" sheetId="2" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="Análise" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <pivotCaches>
+    <pivotCache cacheId="13" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,8 +40,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -49,16 +53,30 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="130">
   <si>
     <t>VendaID</t>
   </si>
@@ -427,6 +445,27 @@
   </si>
   <si>
     <t>9.2 - Filter por Vendas deste mês com a data atual</t>
+  </si>
+  <si>
+    <t>10.1 - Resumo " Região ", " Total ", Nº de Vendas " e " Ticket Médio"</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Sum of Total</t>
+  </si>
+  <si>
+    <t>Sum of Quantidade</t>
+  </si>
+  <si>
+    <t>Médio</t>
+  </si>
+  <si>
+    <t>Baixo</t>
+  </si>
+  <si>
+    <t>Alto</t>
   </si>
 </sst>
 </file>
@@ -568,7 +607,7 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -634,6 +673,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -763,24 +814,1360 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Filipe Matos" refreshedDate="45942.925748148147" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="36" xr:uid="{11D988A2-CAEF-458D-8315-73FCD062F430}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="VEndas"/>
+  </cacheSource>
+  <cacheFields count="22">
+    <cacheField name="VendaID" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Data" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2024-07-21T00:00:00" maxDate="2025-09-18T00:00:00"/>
+    </cacheField>
+    <cacheField name="Ano" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Mês" numFmtId="164">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Fim do Mês" numFmtId="164">
+      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2024-07-31T00:00:00" maxDate="2025-10-01T00:00:00"/>
+    </cacheField>
+    <cacheField name="Trimestre" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="4"/>
+    </cacheField>
+    <cacheField name="Cliente" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Região" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Norte"/>
+        <s v="Lisboa"/>
+        <s v="Centro"/>
+        <s v="Algarve"/>
+        <s v="Alentejo"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Vendedor" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Diogo"/>
+        <s v="Ana"/>
+        <s v="Bruno"/>
+        <s v="Carla"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Categoria" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Papelaria"/>
+        <s v="Eletrónica"/>
+        <s v="Higiene"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Produto" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Quantidade" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="23"/>
+    </cacheField>
+    <cacheField name="PreçoUnitário" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.69" maxValue="36.57"/>
+    </cacheField>
+    <cacheField name="Desconto(%)" numFmtId="9">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="0.15"/>
+    </cacheField>
+    <cacheField name="Total" numFmtId="44">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="6.2729999999999997" maxValue="638.495"/>
+    </cacheField>
+    <cacheField name="DiasDesdeVenda" numFmtId="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="25" maxValue="448"/>
+    </cacheField>
+    <cacheField name="TicketClass" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Baixo"/>
+        <s v="Médio"/>
+        <s v="Alto"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="EscalaCliente" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Bronze"/>
+        <s v="Ouro"/>
+        <s v="Prata"/>
+        <s v="Platina"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="AproxEscalaClienteInf" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="AproxEscalaClienteSup" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Column1" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Column2" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="36">
+  <r>
+    <s v="V008"/>
+    <d v="2024-07-21T00:00:00"/>
+    <s v="2024"/>
+    <s v="07"/>
+    <d v="2024-07-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Alfa Lda"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Caderno A5"/>
+    <n v="13"/>
+    <n v="4.2300000000000004"/>
+    <n v="0.15"/>
+    <n v="46.741500000000009"/>
+    <n v="448"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V031"/>
+    <d v="2024-07-22T00:00:00"/>
+    <s v="2024"/>
+    <s v="07"/>
+    <d v="2024-07-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Epsilon Co."/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Bloco Notas"/>
+    <n v="4"/>
+    <n v="8.24"/>
+    <n v="0"/>
+    <n v="32.96"/>
+    <n v="447"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V035"/>
+    <d v="2024-08-18T00:00:00"/>
+    <s v="2024"/>
+    <s v="08"/>
+    <d v="2024-08-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Alfa Lda"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Papel A4 500"/>
+    <n v="3"/>
+    <n v="4.22"/>
+    <n v="0.05"/>
+    <n v="12.026999999999999"/>
+    <n v="420"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V036"/>
+    <d v="2024-08-28T00:00:00"/>
+    <s v="2024"/>
+    <s v="08"/>
+    <d v="2024-08-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Eta Market"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Papel A4 500"/>
+    <n v="1"/>
+    <n v="7.38"/>
+    <n v="0.15"/>
+    <n v="6.2729999999999997"/>
+    <n v="410"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V006"/>
+    <d v="2024-09-10T00:00:00"/>
+    <s v="2024"/>
+    <s v="09"/>
+    <d v="2024-09-30T00:00:00"/>
+    <n v="3"/>
+    <s v="Theta Super"/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Marcadores"/>
+    <n v="4"/>
+    <n v="11.35"/>
+    <n v="0.05"/>
+    <n v="43.129999999999995"/>
+    <n v="397"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V013"/>
+    <d v="2024-09-26T00:00:00"/>
+    <s v="2024"/>
+    <s v="09"/>
+    <d v="2024-09-30T00:00:00"/>
+    <n v="3"/>
+    <s v="Eta Market"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Bloco Notas"/>
+    <n v="10"/>
+    <n v="6.85"/>
+    <n v="0.1"/>
+    <n v="61.65"/>
+    <n v="381"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V015"/>
+    <d v="2024-10-08T00:00:00"/>
+    <s v="2024"/>
+    <s v="10"/>
+    <d v="2024-10-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Epsilon Co."/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Teclado"/>
+    <n v="2"/>
+    <n v="33.71"/>
+    <n v="0.15"/>
+    <n v="57.307000000000002"/>
+    <n v="369"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V001"/>
+    <d v="2024-10-11T00:00:00"/>
+    <s v="2024"/>
+    <s v="10"/>
+    <d v="2024-10-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Gamma, SA"/>
+    <x v="0"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Luvas Nitrilo"/>
+    <n v="16"/>
+    <n v="3.22"/>
+    <n v="0.15"/>
+    <n v="43.792000000000002"/>
+    <n v="366"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V009"/>
+    <d v="2024-10-11T00:00:00"/>
+    <s v="2024"/>
+    <s v="10"/>
+    <d v="2024-10-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Alfa Lda"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Auricular"/>
+    <n v="8"/>
+    <n v="36.57"/>
+    <n v="0.15"/>
+    <n v="248.67599999999999"/>
+    <n v="366"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Platina"/>
+    <s v="Ouro"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V005"/>
+    <d v="2024-10-15T00:00:00"/>
+    <s v="2024"/>
+    <s v="10"/>
+    <d v="2024-10-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Beta &amp; Filhos"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Marcadores"/>
+    <n v="22"/>
+    <n v="4.57"/>
+    <n v="0.05"/>
+    <n v="95.513000000000005"/>
+    <n v="362"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V010"/>
+    <d v="2024-10-30T00:00:00"/>
+    <s v="2024"/>
+    <s v="10"/>
+    <d v="2024-10-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Eta Market"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Máscaras 50x"/>
+    <n v="10"/>
+    <n v="14.45"/>
+    <n v="0"/>
+    <n v="144.5"/>
+    <n v="347"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V018"/>
+    <d v="2024-11-08T00:00:00"/>
+    <s v="2024"/>
+    <s v="11"/>
+    <d v="2024-11-30T00:00:00"/>
+    <n v="4"/>
+    <s v="Alfa Lda"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Auricular"/>
+    <n v="8"/>
+    <n v="19.28"/>
+    <n v="0.05"/>
+    <n v="146.52799999999999"/>
+    <n v="338"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V019"/>
+    <d v="2024-11-27T00:00:00"/>
+    <s v="2024"/>
+    <s v="11"/>
+    <d v="2024-11-30T00:00:00"/>
+    <n v="4"/>
+    <s v="Delta Unip."/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Luvas Nitrilo"/>
+    <n v="22"/>
+    <n v="7.73"/>
+    <n v="0.1"/>
+    <n v="153.054"/>
+    <n v="319"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V017"/>
+    <d v="2024-11-29T00:00:00"/>
+    <s v="2024"/>
+    <s v="11"/>
+    <d v="2024-11-30T00:00:00"/>
+    <n v="4"/>
+    <s v="Iota Digital"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Toalhitas"/>
+    <n v="1"/>
+    <n v="8.02"/>
+    <n v="0.05"/>
+    <n v="7.6189999999999989"/>
+    <n v="317"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V029"/>
+    <d v="2024-12-08T00:00:00"/>
+    <s v="2024"/>
+    <s v="12"/>
+    <d v="2024-12-31T00:00:00"/>
+    <n v="4"/>
+    <s v="Delta Unip."/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Caderno A5"/>
+    <n v="17"/>
+    <n v="8.1300000000000008"/>
+    <n v="0.1"/>
+    <n v="124.38900000000001"/>
+    <n v="308"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V007"/>
+    <d v="2025-01-05T00:00:00"/>
+    <s v="2025"/>
+    <s v="01"/>
+    <d v="2025-01-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Epsilon Co."/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Marcadores"/>
+    <n v="21"/>
+    <n v="1.69"/>
+    <n v="0.15"/>
+    <n v="30.166499999999999"/>
+    <n v="280"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V026"/>
+    <d v="2025-01-08T00:00:00"/>
+    <s v="2025"/>
+    <s v="01"/>
+    <d v="2025-01-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Gamma, SA"/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Caderno A5"/>
+    <n v="18"/>
+    <n v="8.5"/>
+    <n v="0"/>
+    <n v="153"/>
+    <n v="277"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V011"/>
+    <d v="2025-01-31T00:00:00"/>
+    <s v="2025"/>
+    <s v="01"/>
+    <d v="2025-01-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Gamma, SA"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Powerbank"/>
+    <n v="23"/>
+    <n v="20.239999999999998"/>
+    <n v="0.15"/>
+    <n v="395.69199999999995"/>
+    <n v="254"/>
+    <x v="2"/>
+    <x v="3"/>
+    <e v="#N/A"/>
+    <s v="Platina"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V033"/>
+    <d v="2025-02-21T00:00:00"/>
+    <s v="2025"/>
+    <s v="02"/>
+    <d v="2025-02-28T00:00:00"/>
+    <n v="1"/>
+    <s v="Alfa Lda"/>
+    <x v="2"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Papel A4 500"/>
+    <n v="2"/>
+    <n v="6.46"/>
+    <n v="0.15"/>
+    <n v="10.981999999999999"/>
+    <n v="233"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V032"/>
+    <d v="2025-03-10T00:00:00"/>
+    <s v="2025"/>
+    <s v="03"/>
+    <d v="2025-03-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Eta Market"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="2"/>
+    <s v="Máscaras 50x"/>
+    <n v="16"/>
+    <n v="12.69"/>
+    <n v="0"/>
+    <n v="203.04"/>
+    <n v="216"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Platina"/>
+    <s v="Ouro"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V021"/>
+    <d v="2025-03-15T00:00:00"/>
+    <s v="2025"/>
+    <s v="03"/>
+    <d v="2025-03-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Alfa Lda"/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Teclado"/>
+    <n v="22"/>
+    <n v="30.55"/>
+    <n v="0.05"/>
+    <n v="638.495"/>
+    <n v="211"/>
+    <x v="2"/>
+    <x v="3"/>
+    <e v="#N/A"/>
+    <s v="Platina"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V004"/>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="2025"/>
+    <s v="03"/>
+    <d v="2025-03-31T00:00:00"/>
+    <n v="1"/>
+    <s v="Delta Unip."/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+    <s v="Toalhitas"/>
+    <n v="8"/>
+    <n v="4.3899999999999997"/>
+    <n v="0"/>
+    <n v="35.119999999999997"/>
+    <n v="198"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V028"/>
+    <d v="2025-04-03T00:00:00"/>
+    <s v="2025"/>
+    <s v="04"/>
+    <d v="2025-04-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Delta Unip."/>
+    <x v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Teclado"/>
+    <n v="3"/>
+    <n v="14.98"/>
+    <n v="0"/>
+    <n v="44.94"/>
+    <n v="192"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V024"/>
+    <d v="2025-04-20T00:00:00"/>
+    <s v="2025"/>
+    <s v="04"/>
+    <d v="2025-04-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Gamma, SA"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="Powerbank"/>
+    <n v="3"/>
+    <n v="26.8"/>
+    <n v="0.15"/>
+    <n v="68.34"/>
+    <n v="175"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V020"/>
+    <d v="2025-05-05T00:00:00"/>
+    <s v="2025"/>
+    <s v="05"/>
+    <d v="2025-05-31T00:00:00"/>
+    <n v="2"/>
+    <s v="Alfa Lda"/>
+    <x v="1"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Auricular"/>
+    <n v="7"/>
+    <n v="17.39"/>
+    <n v="0.15"/>
+    <n v="103.4705"/>
+    <n v="160"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V030"/>
+    <d v="2025-05-10T00:00:00"/>
+    <s v="2025"/>
+    <s v="05"/>
+    <d v="2025-05-31T00:00:00"/>
+    <n v="2"/>
+    <s v="Beta &amp; Filhos"/>
+    <x v="3"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Bloco Notas"/>
+    <n v="3"/>
+    <n v="5.22"/>
+    <n v="0"/>
+    <n v="15.66"/>
+    <n v="155"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V012"/>
+    <d v="2025-05-27T00:00:00"/>
+    <s v="2025"/>
+    <s v="05"/>
+    <d v="2025-05-31T00:00:00"/>
+    <n v="2"/>
+    <s v="Epsilon Co."/>
+    <x v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Bloco Notas"/>
+    <n v="5"/>
+    <n v="7.26"/>
+    <n v="0.1"/>
+    <n v="32.67"/>
+    <n v="138"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V022"/>
+    <d v="2025-06-09T00:00:00"/>
+    <s v="2025"/>
+    <s v="06"/>
+    <d v="2025-06-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Theta Super"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Luvas Nitrilo"/>
+    <n v="6"/>
+    <n v="10.73"/>
+    <n v="0.05"/>
+    <n v="61.160999999999994"/>
+    <n v="125"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V034"/>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="2025"/>
+    <s v="06"/>
+    <d v="2025-06-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Alfa Lda"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="Powerbank"/>
+    <n v="4"/>
+    <n v="34.729999999999997"/>
+    <n v="0.1"/>
+    <n v="125.02799999999999"/>
+    <n v="124"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V003"/>
+    <d v="2025-06-14T00:00:00"/>
+    <s v="2025"/>
+    <s v="06"/>
+    <d v="2025-06-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Beta &amp; Filhos"/>
+    <x v="2"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Marcadores"/>
+    <n v="18"/>
+    <n v="11.38"/>
+    <n v="0.05"/>
+    <n v="194.59799999999998"/>
+    <n v="120"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V016"/>
+    <d v="2025-06-25T00:00:00"/>
+    <s v="2025"/>
+    <s v="06"/>
+    <d v="2025-06-30T00:00:00"/>
+    <n v="2"/>
+    <s v="Kappa Print"/>
+    <x v="4"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Marcadores"/>
+    <n v="20"/>
+    <n v="9.8800000000000008"/>
+    <n v="0.15"/>
+    <n v="167.96"/>
+    <n v="109"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V014"/>
+    <d v="2025-07-08T00:00:00"/>
+    <s v="2025"/>
+    <s v="07"/>
+    <d v="2025-07-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Delta Unip."/>
+    <x v="0"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Powerbank"/>
+    <n v="5"/>
+    <n v="28.84"/>
+    <n v="0.15"/>
+    <n v="122.57"/>
+    <n v="96"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Ouro"/>
+    <s v="Prata"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V025"/>
+    <d v="2025-07-21T00:00:00"/>
+    <s v="2025"/>
+    <s v="07"/>
+    <d v="2025-07-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Eta Market"/>
+    <x v="0"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Bloco Notas"/>
+    <n v="7"/>
+    <n v="9.94"/>
+    <n v="0.15"/>
+    <n v="59.142999999999994"/>
+    <n v="83"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V023"/>
+    <d v="2025-08-18T00:00:00"/>
+    <s v="2025"/>
+    <s v="08"/>
+    <d v="2025-08-31T00:00:00"/>
+    <n v="3"/>
+    <s v="Alfa Lda"/>
+    <x v="1"/>
+    <x v="3"/>
+    <x v="2"/>
+    <s v="Álcool Gel"/>
+    <n v="5"/>
+    <n v="13.79"/>
+    <n v="0.15"/>
+    <n v="58.607499999999987"/>
+    <n v="55"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V002"/>
+    <d v="2025-09-09T00:00:00"/>
+    <s v="2025"/>
+    <s v="09"/>
+    <d v="2025-09-30T00:00:00"/>
+    <n v="3"/>
+    <s v="Eta Market"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Toalhitas"/>
+    <n v="5"/>
+    <n v="11.68"/>
+    <n v="0.1"/>
+    <n v="52.56"/>
+    <n v="33"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <s v="V027"/>
+    <d v="2025-09-17T00:00:00"/>
+    <s v="2025"/>
+    <s v="09"/>
+    <d v="2025-09-30T00:00:00"/>
+    <n v="3"/>
+    <s v="Epsilon Co."/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+    <s v="Toalhitas"/>
+    <n v="20"/>
+    <n v="5.21"/>
+    <n v="0.15"/>
+    <n v="88.57"/>
+    <n v="25"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Prata"/>
+    <s v="Bronze"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7DDDDEFE-87A1-41B2-87EA-64FBCFD781FC}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="W24:Y60" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="22">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="8"/>
+    <field x="9"/>
+    <field x="16"/>
+  </rowFields>
+  <rowItems count="36">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="14" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Sum of Quantidade" fld="11" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E5A8D4A9-AB62-4DBD-BF43-6765046C9CA9}" name="PivotTable2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="W4:Y21" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="22">
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField dataField="1" numFmtId="44" showAll="0"/>
+    <pivotField numFmtId="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="7"/>
+    <field x="17"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Sum of Total" fld="14" baseField="0" baseItem="0" numFmtId="44"/>
+    <dataField name="Sum of Quantidade" fld="11" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}" name="Vendas" displayName="Vendas" ref="A1:V37" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:V37" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="Norte"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="9">
-      <filters>
-        <filter val="Higiene"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:V37" xr:uid="{A707BE66-5A23-4B3D-AE9F-A76AEC8A8611}"/>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00E18295-A8E0-4DEE-A175-C2D1DE60A124}" name="VendaID" dataDxfId="21"/>
     <tableColumn id="2" xr3:uid="{2A9F5B6B-8F27-432C-B2C7-24A3E549C555}" name="Data" dataDxfId="20"/>
@@ -1222,11 +2609,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V40"/>
   <sheetViews>
-    <sheetView topLeftCell="J2" workbookViewId="0">
+    <sheetView topLeftCell="J9" workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1307,7 +2694,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>10</v>
       </c>
@@ -1360,7 +2747,7 @@
       </c>
       <c r="P2" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1381,7 +2768,7 @@
       <c r="U2" s="10"/>
       <c r="V2" s="10"/>
     </row>
-    <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -1434,7 +2821,7 @@
       </c>
       <c r="P3" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="Q3" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1455,7 +2842,7 @@
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
     </row>
-    <row r="4" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -1508,7 +2895,7 @@
       </c>
       <c r="P4" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="Q4" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1529,7 +2916,7 @@
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
     </row>
-    <row r="5" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -1582,7 +2969,7 @@
       </c>
       <c r="P5" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="Q5" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1603,7 +2990,7 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
     </row>
-    <row r="6" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
@@ -1656,7 +3043,7 @@
       </c>
       <c r="P6" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="Q6" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1677,7 +3064,7 @@
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
     </row>
-    <row r="7" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
@@ -1730,7 +3117,7 @@
       </c>
       <c r="P7" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="Q7" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1751,7 +3138,7 @@
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
     </row>
-    <row r="8" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
@@ -1804,7 +3191,7 @@
       </c>
       <c r="P8" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="Q8" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1878,7 +3265,7 @@
       </c>
       <c r="P9" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="Q9" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1899,7 +3286,7 @@
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
     </row>
-    <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>38</v>
       </c>
@@ -1952,7 +3339,7 @@
       </c>
       <c r="P10" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="Q10" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -1973,7 +3360,7 @@
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
     </row>
-    <row r="11" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>40</v>
       </c>
@@ -2026,7 +3413,7 @@
       </c>
       <c r="P11" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="Q11" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2047,7 +3434,7 @@
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
     </row>
-    <row r="12" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>42</v>
       </c>
@@ -2100,7 +3487,7 @@
       </c>
       <c r="P12" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="Q12" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2121,7 +3508,7 @@
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
     </row>
-    <row r="13" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>44</v>
       </c>
@@ -2174,7 +3561,7 @@
       </c>
       <c r="P13" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="Q13" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2248,7 +3635,7 @@
       </c>
       <c r="P14" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="Q14" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2269,7 +3656,7 @@
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
     </row>
-    <row r="15" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>48</v>
       </c>
@@ -2322,7 +3709,7 @@
       </c>
       <c r="P15" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="Q15" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2343,7 +3730,7 @@
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
     </row>
-    <row r="16" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>51</v>
       </c>
@@ -2396,7 +3783,7 @@
       </c>
       <c r="P16" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="Q16" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2417,7 +3804,7 @@
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
     </row>
-    <row r="17" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>52</v>
       </c>
@@ -2470,7 +3857,7 @@
       </c>
       <c r="P17" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="Q17" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2491,7 +3878,7 @@
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
     </row>
-    <row r="18" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>53</v>
       </c>
@@ -2544,7 +3931,7 @@
       </c>
       <c r="P18" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="Q18" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2565,7 +3952,7 @@
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
     </row>
-    <row r="19" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>55</v>
       </c>
@@ -2618,7 +4005,7 @@
       </c>
       <c r="P19" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="Q19" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2639,7 +4026,7 @@
       <c r="U19" s="10"/>
       <c r="V19" s="10"/>
     </row>
-    <row r="20" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>57</v>
       </c>
@@ -2692,7 +4079,7 @@
       </c>
       <c r="P20" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="Q20" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2766,7 +4153,7 @@
       </c>
       <c r="P21" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="Q21" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2787,7 +4174,7 @@
       <c r="U21" s="10"/>
       <c r="V21" s="10"/>
     </row>
-    <row r="22" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>59</v>
       </c>
@@ -2840,7 +4227,7 @@
       </c>
       <c r="P22" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="Q22" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2914,7 +4301,7 @@
       </c>
       <c r="P23" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="Q23" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -2935,7 +4322,7 @@
       <c r="U23" s="10"/>
       <c r="V23" s="10"/>
     </row>
-    <row r="24" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>61</v>
       </c>
@@ -2988,7 +4375,7 @@
       </c>
       <c r="P24" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="Q24" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3009,7 +4396,7 @@
       <c r="U24" s="10"/>
       <c r="V24" s="10"/>
     </row>
-    <row r="25" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>62</v>
       </c>
@@ -3062,7 +4449,7 @@
       </c>
       <c r="P25" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="Q25" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3083,7 +4470,7 @@
       <c r="U25" s="10"/>
       <c r="V25" s="10"/>
     </row>
-    <row r="26" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>63</v>
       </c>
@@ -3136,7 +4523,7 @@
       </c>
       <c r="P26" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="Q26" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3157,7 +4544,7 @@
       <c r="U26" s="10"/>
       <c r="V26" s="10"/>
     </row>
-    <row r="27" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>64</v>
       </c>
@@ -3210,7 +4597,7 @@
       </c>
       <c r="P27" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="Q27" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3231,7 +4618,7 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
     </row>
-    <row r="28" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>65</v>
       </c>
@@ -3284,7 +4671,7 @@
       </c>
       <c r="P28" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Q28" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3358,7 +4745,7 @@
       </c>
       <c r="P29" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="Q29" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3379,7 +4766,7 @@
       <c r="U29" s="10"/>
       <c r="V29" s="10"/>
     </row>
-    <row r="30" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>67</v>
       </c>
@@ -3432,7 +4819,7 @@
       </c>
       <c r="P30" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="Q30" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3453,7 +4840,7 @@
       <c r="U30" s="10"/>
       <c r="V30" s="10"/>
     </row>
-    <row r="31" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>68</v>
       </c>
@@ -3506,7 +4893,7 @@
       </c>
       <c r="P31" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="Q31" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3527,7 +4914,7 @@
       <c r="U31" s="10"/>
       <c r="V31" s="10"/>
     </row>
-    <row r="32" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="10" t="s">
         <v>69</v>
       </c>
@@ -3580,7 +4967,7 @@
       </c>
       <c r="P32" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="Q32" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3601,7 +4988,7 @@
       <c r="U32" s="10"/>
       <c r="V32" s="10"/>
     </row>
-    <row r="33" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>72</v>
       </c>
@@ -3654,7 +5041,7 @@
       </c>
       <c r="P33" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="Q33" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3675,7 +5062,7 @@
       <c r="U33" s="10"/>
       <c r="V33" s="10"/>
     </row>
-    <row r="34" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>73</v>
       </c>
@@ -3728,7 +5115,7 @@
       </c>
       <c r="P34" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="Q34" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3749,7 +5136,7 @@
       <c r="U34" s="10"/>
       <c r="V34" s="10"/>
     </row>
-    <row r="35" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>74</v>
       </c>
@@ -3802,7 +5189,7 @@
       </c>
       <c r="P35" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="Q35" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3823,7 +5210,7 @@
       <c r="U35" s="10"/>
       <c r="V35" s="10"/>
     </row>
-    <row r="36" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>76</v>
       </c>
@@ -3876,7 +5263,7 @@
       </c>
       <c r="P36" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="Q36" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3897,7 +5284,7 @@
       <c r="U36" s="10"/>
       <c r="V36" s="10"/>
     </row>
-    <row r="37" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>77</v>
       </c>
@@ -3950,7 +5337,7 @@
       </c>
       <c r="P37" s="16">
         <f ca="1">VALUE(TODAY()-Vendas[[#This Row],[Data]])</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Q37" s="10" t="str">
         <f>IF(Vendas[[#This Row],[Total]]&gt;=250,"Alto", IF(AND(Vendas[[#This Row],[Total]]&gt;=100,Vendas[[#This Row],[Total]]&lt;=249.99),"Médio","Baixo"))</f>
@@ -3985,10 +5372,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D0DA00-7E98-40C2-8941-409BD587D4AF}">
-  <dimension ref="B2:S28"/>
+  <dimension ref="B2:Y60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -4001,9 +5388,13 @@
     <col min="10" max="10" width="32" customWidth="1"/>
     <col min="11" max="13" width="20.5703125" customWidth="1"/>
     <col min="17" max="17" width="25.140625" customWidth="1"/>
+    <col min="18" max="19" width="12.28515625" customWidth="1"/>
+    <col min="23" max="23" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="26.140625" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:25" ht="45" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>90</v>
       </c>
@@ -4016,8 +5407,11 @@
       <c r="Q2" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W2" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>19</v>
       </c>
@@ -4050,8 +5444,9 @@
       <c r="S3" s="9" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W3" s="3"/>
+    </row>
+    <row r="4" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>25</v>
       </c>
@@ -4087,8 +5482,17 @@
       <c r="S4" s="10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W4" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="X4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>47</v>
       </c>
@@ -4124,8 +5528,17 @@
       <c r="S5" s="10" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W5" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="X5" s="26">
+        <v>167.96</v>
+      </c>
+      <c r="Y5" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -4161,8 +5574,17 @@
       <c r="S6" s="10" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W6" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X6" s="26">
+        <v>167.96</v>
+      </c>
+      <c r="Y6" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F7" s="5"/>
       <c r="R7" s="10">
         <v>350</v>
@@ -4170,11 +5592,29 @@
       <c r="S7" s="10" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W7" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="X7" s="26">
+        <v>201.32999999999998</v>
+      </c>
+      <c r="Y7" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="W8" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="X8" s="26">
+        <v>48.33</v>
+      </c>
+      <c r="Y8" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>91</v>
       </c>
@@ -4187,8 +5627,17 @@
       <c r="Q9" s="4" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W9" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X9" s="26">
+        <v>153</v>
+      </c>
+      <c r="Y9" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>71</v>
       </c>
@@ -4215,8 +5664,17 @@
       <c r="M10" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W10" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="X10" s="26">
+        <v>845.20749999999987</v>
+      </c>
+      <c r="Y10" s="27">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>54</v>
       </c>
@@ -4244,8 +5702,17 @@
         <f t="array" ref="Q11:Q15">_xlfn._xlws.FILTER(Vendas[Quantidade],((Vendas[Categoria]="Higiene")*(Vendas[Região]="Norte")))</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W11" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="X11" s="26">
+        <v>110.41749999999999</v>
+      </c>
+      <c r="Y11" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
@@ -4272,8 +5739,17 @@
       <c r="Q12" s="21">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W12" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X12" s="26">
+        <v>395.69199999999995</v>
+      </c>
+      <c r="Y12" s="27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
@@ -4300,8 +5776,17 @@
       <c r="Q13" s="21">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W13" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X13" s="26">
+        <v>339.09799999999996</v>
+      </c>
+      <c r="Y13" s="27">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>12</v>
       </c>
@@ -4313,18 +5798,45 @@
       <c r="Q14" s="21">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W14" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="X14" s="26">
+        <v>803.95299999999997</v>
+      </c>
+      <c r="Y14" s="27">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F15" s="5"/>
       <c r="Q15" s="21">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="W15" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="X15" s="26">
+        <v>553.95449999999994</v>
+      </c>
+      <c r="Y15" s="27">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F16" s="5"/>
       <c r="Q16" s="21"/>
-    </row>
-    <row r="17" spans="2:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="W16" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X16" s="26">
+        <v>249.99849999999998</v>
+      </c>
+      <c r="Y16" s="27">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>92</v>
       </c>
@@ -4332,8 +5844,17 @@
         <v>96</v>
       </c>
       <c r="Q17" s="21"/>
-    </row>
-    <row r="18" spans="2:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="W17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="X17" s="26">
+        <v>1867.4824999999998</v>
+      </c>
+      <c r="Y17" s="27">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:25" ht="45" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>32</v>
       </c>
@@ -4351,8 +5872,17 @@
       <c r="Q18" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W18" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="X18" s="26">
+        <v>252.23050000000001</v>
+      </c>
+      <c r="Y18" s="27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>36</v>
       </c>
@@ -4362,8 +5892,17 @@
       </c>
       <c r="F19" s="5"/>
       <c r="Q19" s="21"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W19" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="X19" s="26">
+        <v>451.71600000000001</v>
+      </c>
+      <c r="Y19" s="27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -4372,31 +5911,449 @@
         <v>67.928937499999989</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="Q20" s="21"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q20" s="10" t="e" cm="1" vm="1">
+        <f t="array" aca="1" ref="Q20" ca="1">_xlfn._xlws.FILTER(Vendas[Quantidade],(MONTH(Vendas[Data])=(MONTH(TODAY())))*(YEAR(Vendas[Data])=(YEAR(TODAY()))))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W20" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="X20" s="26">
+        <v>638.495</v>
+      </c>
+      <c r="Y20" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q21" s="21"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W21" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="X21" s="26">
+        <v>525.04099999999994</v>
+      </c>
+      <c r="Y21" s="27">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q22" s="21"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q23" s="21"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q24" s="21"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W24" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="X24" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q25" s="21"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W25" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="X25" s="26">
+        <v>817.27649999999994</v>
+      </c>
+      <c r="Y25" s="27">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q26" s="21"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W26" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="X26" s="26">
+        <v>57.307000000000002</v>
+      </c>
+      <c r="Y26" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q27" s="21"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="W27" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X27" s="26">
+        <v>57.307000000000002</v>
+      </c>
+      <c r="Y27" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
       <c r="Q28" s="21"/>
+      <c r="W28" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="X28" s="26">
+        <v>329.42200000000003</v>
+      </c>
+      <c r="Y28" s="27">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W29" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X29" s="26">
+        <v>184.922</v>
+      </c>
+      <c r="Y29" s="27">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W30" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X30" s="26">
+        <v>144.5</v>
+      </c>
+      <c r="Y30" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W31" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="X31" s="26">
+        <v>430.54749999999996</v>
+      </c>
+      <c r="Y31" s="27">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W32" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X32" s="26">
+        <v>235.94949999999997</v>
+      </c>
+      <c r="Y32" s="27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W33" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X33" s="26">
+        <v>194.59799999999998</v>
+      </c>
+      <c r="Y33" s="27">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W34" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="X34" s="26">
+        <v>1784.0284999999997</v>
+      </c>
+      <c r="Y34" s="27">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W35" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="X35" s="26">
+        <v>1406.7554999999998</v>
+      </c>
+      <c r="Y35" s="27">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W36" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="X36" s="26">
+        <v>1034.1869999999999</v>
+      </c>
+      <c r="Y36" s="27">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W37" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X37" s="26">
+        <v>372.56849999999997</v>
+      </c>
+      <c r="Y37" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W38" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="X38" s="26">
+        <v>203.04</v>
+      </c>
+      <c r="Y38" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W39" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X39" s="26">
+        <v>203.04</v>
+      </c>
+      <c r="Y39" s="27">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W40" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="X40" s="26">
+        <v>174.233</v>
+      </c>
+      <c r="Y40" s="27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W41" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X41" s="26">
+        <v>6.2729999999999997</v>
+      </c>
+      <c r="Y41" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W42" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X42" s="26">
+        <v>167.96</v>
+      </c>
+      <c r="Y42" s="27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W43" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="X43" s="26">
+        <v>543.93449999999996</v>
+      </c>
+      <c r="Y43" s="27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W44" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="X44" s="26">
+        <v>193.36799999999999</v>
+      </c>
+      <c r="Y44" s="27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W45" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X45" s="26">
+        <v>68.34</v>
+      </c>
+      <c r="Y45" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W46" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X46" s="26">
+        <v>125.02799999999999</v>
+      </c>
+      <c r="Y46" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W47" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="X47" s="26">
+        <v>280.44149999999996</v>
+      </c>
+      <c r="Y47" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W48" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X48" s="26">
+        <v>127.38749999999997</v>
+      </c>
+      <c r="Y48" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W49" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X49" s="26">
+        <v>153.054</v>
+      </c>
+      <c r="Y49" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W50" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="X50" s="26">
+        <v>70.125</v>
+      </c>
+      <c r="Y50" s="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W51" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X51" s="26">
+        <v>70.125</v>
+      </c>
+      <c r="Y51" s="27">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W52" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="X52" s="26">
+        <v>740.69350000000009</v>
+      </c>
+      <c r="Y52" s="27">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="53" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W53" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="X53" s="26">
+        <v>293.61599999999999</v>
+      </c>
+      <c r="Y53" s="27">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W54" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X54" s="26">
+        <v>44.94</v>
+      </c>
+      <c r="Y54" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W55" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X55" s="26">
+        <v>248.67599999999999</v>
+      </c>
+      <c r="Y55" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W56" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="X56" s="26">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="Y56" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W57" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X57" s="26">
+        <v>35.119999999999997</v>
+      </c>
+      <c r="Y57" s="27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W58" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="X58" s="26">
+        <v>411.95750000000004</v>
+      </c>
+      <c r="Y58" s="27">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W59" s="29" t="s">
+        <v>128</v>
+      </c>
+      <c r="X59" s="26">
+        <v>134.56850000000003</v>
+      </c>
+      <c r="Y59" s="27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="23:25" x14ac:dyDescent="0.25">
+      <c r="W60" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="X60" s="26">
+        <v>277.38900000000001</v>
+      </c>
+      <c r="Y60" s="27">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>